<commit_message>
Exporting metrics for each files in the analysed project (#30)
</commit_message>
<xml_diff>
--- a/src/main/resources/template/issues-template.xlsx
+++ b/src/main/resources/template/issues-template.xlsx
@@ -1,32 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\begarco\cnesreport\sonar-cnes-report\src\main\resources\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\labo\IdeaProjects\sonar-cnes-report\src\main\resources\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:80001_{A8D77D61-0A09-4B30-9961-DFF5D9114F6E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="750" yWindow="510" windowWidth="13815" windowHeight="5835" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TCD" sheetId="3" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
     <sheet name="All" sheetId="2" r:id="rId3"/>
     <sheet name="Unconfirmed" sheetId="4" r:id="rId4"/>
+    <sheet name="Metrics" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId5"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>Rule</t>
   </si>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -623,7 +623,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="4" formatCode="#,##0.00"/>
     </dxf>
@@ -653,11 +656,11 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Benoît Garçon" refreshedDate="43374.037758796294" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF27000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="labo" refreshedDate="43571.447895833335" createdVersion="4" refreshedVersion="6" minRefreshableVersion="3" recordCount="1">
   <cacheSource type="worksheet">
     <worksheetSource name="selected"/>
   </cacheSource>
-  <cacheFields count="9">
+  <cacheFields count="10">
     <cacheField name="Rule" numFmtId="0">
       <sharedItems containsNonDate="0" containsBlank="1" count="6">
         <m/>
@@ -708,6 +711,9 @@
     <cacheField name="Status" numFmtId="0">
       <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
     </cacheField>
+    <cacheField name="Comments" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -718,7 +724,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -729,14 +735,15 @@
     <m/>
     <m/>
     <m/>
+    <m/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="synthesis" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="synthesis" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="9">
+  <pivotFields count="10">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item m="1" x="1"/>
@@ -781,6 +788,7 @@
     </pivotField>
     <pivotField showAll="0"/>
     <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
     <pivotField showAll="0" defaultSubtotal="0"/>
   </pivotFields>
@@ -830,48 +838,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="selected" displayName="selected" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:J2"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Rule"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Message" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Severity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Language"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="File"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Line"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Effort"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Status"/>
-    <tableColumn id="10" xr3:uid="{ECD7FBFF-2911-43D1-A7B1-9BD75AE9511A}" name="Comments"/>
+    <tableColumn id="1" name="Rule"/>
+    <tableColumn id="2" name="Message" dataDxfId="4"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Severity"/>
+    <tableColumn id="8" name="Language"/>
+    <tableColumn id="5" name="File"/>
+    <tableColumn id="6" name="Line"/>
+    <tableColumn id="7" name="Effort"/>
+    <tableColumn id="9" name="Status"/>
+    <tableColumn id="10" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:A2" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="all" displayName="all" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="A1:A2"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Colonne1"/>
+    <tableColumn id="1" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:J2" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="unconfirmed" displayName="unconfirmed" ref="A1:J2" insertRow="1" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="A1:J2"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Rule"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Message" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Type"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Severity"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Language"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="File"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Line"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Effort"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Status"/>
-    <tableColumn id="10" xr3:uid="{2C6AAEB9-4103-4F44-A14E-E358A5B26A34}" name="Comments"/>
+    <tableColumn id="1" name="Rule"/>
+    <tableColumn id="2" name="Message" dataDxfId="1"/>
+    <tableColumn id="3" name="Type"/>
+    <tableColumn id="4" name="Severity"/>
+    <tableColumn id="8" name="Language"/>
+    <tableColumn id="5" name="File"/>
+    <tableColumn id="6" name="Line"/>
+    <tableColumn id="7" name="Effort"/>
+    <tableColumn id="9" name="Status"/>
+    <tableColumn id="10" name="Comments"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="metrics" displayName="metrics" ref="A1:A2" insertRow="1" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:A2"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Colonne1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -953,23 +971,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1005,23 +1006,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1197,11 +1181,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="pivotTable"/>
   <dimension ref="A3:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1261,7 +1245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="selectedIssues"/>
   <dimension ref="A1:J3"/>
   <sheetViews>
@@ -1325,7 +1309,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="allIssues"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1358,7 +1342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1419,4 +1403,34 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>